<commit_message>
Funcionamiento correcto del histograma
</commit_message>
<xml_diff>
--- a/gen_excel/tableros_concurso_.xlsx
+++ b/gen_excel/tableros_concurso_.xlsx
@@ -417,10 +417,10 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Opcion para restablecer concurso
-Limpia el concurso
-Los log de ronda
-Tableros y puntajes
-Genere de nuevo preguntas aleatorias
</commit_message>
<xml_diff>
--- a/gen_excel/tableros_concurso_.xlsx
+++ b/gen_excel/tableros_concurso_.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
   <si>
     <t>RONDA</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>PUNTAJE</t>
+  </si>
+  <si>
+    <t>RONDA EMPATE</t>
   </si>
 </sst>
 </file>
@@ -390,7 +393,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -398,7 +401,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -422,6 +425,9 @@
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>